<commit_message>
Implemented 'Nearest Four Neighbors' mutation
</commit_message>
<xml_diff>
--- a/dataset/P_8_N_72.xlsx
+++ b/dataset/P_8_N_72.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luker\source\repos\EC_P-Median\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB3FD00-5967-4338-9C70-293EC540274D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA5852C-3D4E-4CCD-BE7F-427141EDE24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4956" yWindow="1032" windowWidth="17280" windowHeight="8994" xr2:uid="{5E41DCFD-76F7-4443-88D2-FFFE78AF4D78}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>